<commit_message>
adding new required field "location" to the demands in the cookbook spreadsheets
</commit_message>
<xml_diff>
--- a/doc/cookbook/calendar/calendar-working-hours.xlsx
+++ b/doc/cookbook/calendar/calendar-working-hours.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="135" yWindow="563" windowWidth="22718" windowHeight="11055" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="135" yWindow="563" windowWidth="22718" windowHeight="11055" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="buffer" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14037" uniqueCount="6472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14039" uniqueCount="6472">
   <si>
     <t>name</t>
   </si>
@@ -20189,15 +20189,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20205,19 +20205,22 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -20225,15 +20228,18 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10</v>
       </c>
     </row>
@@ -20339,7 +20345,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -20442,7 +20448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3484"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>